<commit_message>
Added Extent Reports and Error Handling
</commit_message>
<xml_diff>
--- a/TestData/TestDataBoonSupply.xlsx
+++ b/TestData/TestDataBoonSupply.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C6CF61-E1BD-47E0-BDBB-E879135787CE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121A1D17-F38D-4E8B-8619-5E6407F4E31A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario4" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="68">
   <si>
     <t>Username</t>
   </si>
@@ -192,21 +192,9 @@
     <t>9989099878</t>
   </si>
   <si>
-    <t>Dwayne</t>
-  </si>
-  <si>
     <t>dwaynewade@getnada.com</t>
   </si>
   <si>
-    <t>dwaynejohn@getnada.com</t>
-  </si>
-  <si>
-    <t>dwaynescott@getnada.com</t>
-  </si>
-  <si>
-    <t>dwaynejhonson@getnada.com</t>
-  </si>
-  <si>
     <t>October</t>
   </si>
   <si>
@@ -226,6 +214,21 @@
   </si>
   <si>
     <t>21</t>
+  </si>
+  <si>
+    <t>Mitchell</t>
+  </si>
+  <si>
+    <t>mitchellwade@getnada.com</t>
+  </si>
+  <si>
+    <t>mitchelljohn@getnada.com</t>
+  </si>
+  <si>
+    <t>mitchellscott@getnada.com</t>
+  </si>
+  <si>
+    <t>mitchelljhonson@getnada.com</t>
   </si>
 </sst>
 </file>
@@ -613,15 +616,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC040C3B-FCF1-4270-916E-08D15E01289B}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -641,10 +644,20 @@
         <v>45</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{B67B0354-858D-4182-B815-B95B9453AF94}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{060B6B7C-A9D2-4F88-A8A3-3854BD6F8063}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{199E29E2-F3FE-4580-BC17-1502FFA7364C}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{E827222D-6FC2-443D-8177-6E2F8C466F43}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -774,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +894,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>50</v>
@@ -890,7 +903,7 @@
         <v>54</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>35</v>
@@ -917,16 +930,16 @@
         <v>30</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="Q2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>24</v>
@@ -952,7 +965,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>51</v>
@@ -961,7 +974,7 @@
         <v>9989099879</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>35</v>
@@ -988,16 +1001,16 @@
         <v>30</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>36</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>24</v>
@@ -1023,7 +1036,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>52</v>
@@ -1032,7 +1045,7 @@
         <v>9989099881</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>35</v>
@@ -1062,7 +1075,7 @@
         <v>36</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>37</v>
@@ -1094,7 +1107,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>53</v>
@@ -1103,7 +1116,7 @@
         <v>9989099881</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>35</v>
@@ -1133,13 +1146,13 @@
         <v>36</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>24</v>
@@ -1162,9 +1175,9 @@
     <hyperlink ref="G2" r:id="rId1" display="random@123" xr:uid="{FD66CD59-B76C-446B-979E-53A81CA85CE0}"/>
     <hyperlink ref="G3:G5" r:id="rId2" display="random@123" xr:uid="{38D92D11-9123-4F02-9DA1-FC9FEA710617}"/>
     <hyperlink ref="F2" r:id="rId3" xr:uid="{EC6DF31C-8E09-4752-81CC-A49DE18839EF}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{6592B837-FD5D-478F-A4E1-A05F723B9F76}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{D5ADACF1-5F83-4AA6-B450-D2C0C3D0642F}"/>
-    <hyperlink ref="F5" r:id="rId6" xr:uid="{B7A97333-6CDA-4761-A842-7959F2036E6E}"/>
+    <hyperlink ref="F3" r:id="rId4" display="dwaynejohn@getnada.com" xr:uid="{6592B837-FD5D-478F-A4E1-A05F723B9F76}"/>
+    <hyperlink ref="F4" r:id="rId5" display="dwaynescott@getnada.com" xr:uid="{D5ADACF1-5F83-4AA6-B450-D2C0C3D0642F}"/>
+    <hyperlink ref="F5" r:id="rId6" display="dwaynejhonson@getnada.com" xr:uid="{B7A97333-6CDA-4761-A842-7959F2036E6E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -1209,7 +1222,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>35</v>
@@ -1223,7 +1236,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>35</v>
@@ -1237,7 +1250,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>35</v>
@@ -1251,7 +1264,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>35</v>
@@ -1259,12 +1272,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="random@123" xr:uid="{7F70F506-7EB4-4DE5-BDC1-76C9992B1535}"/>
-    <hyperlink ref="D3:D5" r:id="rId2" display="random@123" xr:uid="{36F2FB63-20DD-4CD1-8795-F9076142F53F}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{D84EAE84-6DDE-4A3F-AA1D-2366F54A01F2}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{33F4725A-8B0F-49DA-83DA-F2BC5F997A09}"/>
-    <hyperlink ref="C4" r:id="rId5" xr:uid="{3C7A4C85-A06B-4E78-AE56-E66D4FFA5965}"/>
-    <hyperlink ref="C5" r:id="rId6" xr:uid="{7BC31F86-FA4E-42D3-93FB-3F620543C820}"/>
+    <hyperlink ref="D2" r:id="rId1" display="random@123" xr:uid="{C09BBEF7-B0CF-4A61-B4EC-5923F9FBEC2C}"/>
+    <hyperlink ref="D3:D5" r:id="rId2" display="random@123" xr:uid="{A630CAAA-B967-4A15-975C-8080B818EFF7}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{082F0772-4771-4F68-9090-425C067A4C76}"/>
+    <hyperlink ref="C3" r:id="rId4" display="dwaynejohn@getnada.com" xr:uid="{77C94718-2369-4065-8B8B-4452389D3B1F}"/>
+    <hyperlink ref="C4" r:id="rId5" display="dwaynescott@getnada.com" xr:uid="{5696CC73-BD33-42A9-A559-7108D719AC65}"/>
+    <hyperlink ref="C5" r:id="rId6" display="dwaynejhonson@getnada.com" xr:uid="{5D61F5DB-003D-4455-8D21-38502C2C277F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1275,7 +1288,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C2" sqref="C2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,7 +1321,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>35</v>
@@ -1322,7 +1335,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>35</v>
@@ -1336,7 +1349,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>35</v>
@@ -1350,7 +1363,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>35</v>
@@ -1358,12 +1371,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="random@123" xr:uid="{1A5D84E3-D3D1-4F9E-A5DD-2C5B3A50B3A6}"/>
-    <hyperlink ref="D3:D5" r:id="rId2" display="random@123" xr:uid="{16891158-4D24-425A-980C-669BD0A9E27F}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{558965CB-9FBE-4C76-8C6E-953BD6867B7C}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{38677846-BDD0-4385-8D0C-6DBE82BFE692}"/>
-    <hyperlink ref="C4" r:id="rId5" xr:uid="{8B8EEB81-A38A-47F5-891D-0F1BC6CAD97B}"/>
-    <hyperlink ref="C5" r:id="rId6" xr:uid="{CF49A715-BEE1-4848-A75F-3D6DB22390AF}"/>
+    <hyperlink ref="D2" r:id="rId1" display="random@123" xr:uid="{28015F14-ED6D-4FC8-A182-50C797A9B975}"/>
+    <hyperlink ref="D3:D5" r:id="rId2" display="random@123" xr:uid="{6E148373-3458-43C9-BD78-9A9522E74246}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{5368C4AA-1882-4874-BB5C-082F90F5404E}"/>
+    <hyperlink ref="C3" r:id="rId4" display="dwaynejohn@getnada.com" xr:uid="{7C360D37-1EBB-41DC-9312-91C972F12FA1}"/>
+    <hyperlink ref="C4" r:id="rId5" display="dwaynescott@getnada.com" xr:uid="{3399D8C3-C6E8-4B02-8BFC-121A119AC7FD}"/>
+    <hyperlink ref="C5" r:id="rId6" display="dwaynejhonson@getnada.com" xr:uid="{D28DE1B6-4DA1-49CB-B4BF-8C449E093280}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>